<commit_message>
Implemented DDT with List of Maps
</commit_message>
<xml_diff>
--- a/src/test/resources/login.xlsx
+++ b/src/test/resources/login.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salma\IdeaProjects\My_TestNG-project\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504A2544-D465-48DE-A600-DB17066A0325}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67596B65-1615-4F10-A28B-A05A26DD47FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="details" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Your username is invalid!</t>
+  </si>
+  <si>
+    <t>mamed</t>
+  </si>
+  <si>
+    <t>xiyarovic</t>
   </si>
 </sst>
 </file>
@@ -111,6 +117,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -130,7 +204,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -385,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -453,6 +527,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>